<commit_message>
Stanza French Librabries Added
</commit_message>
<xml_diff>
--- a/demo/demo_output/context_visualized.xlsx
+++ b/demo/demo_output/context_visualized.xlsx
@@ -404,27 +404,27 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>patriotisme,économique,jamais,mis,œuvre</t>
+          <t>PME,met,place,patriotisme,économique</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>mis en œuvre</t>
+          <t>un patriotisme économique</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>le protectionnisme intelligent</t>
+          <t>un protectionnisme intelligent</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>la défiscalisation de</t>
+          <t>il dit à</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>défiscalisation,heures,supplémentaires,suppression</t>
+          <t>dit,constructeurs,américains,voulez</t>
         </is>
       </c>
     </row>
@@ -434,27 +434,27 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>mettre,œuvre,protectionnisme,intelligent,mettre</t>
+          <t>patriotisme,économique,jamais,mis,œuvre</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>en avant de</t>
+          <t>mis en œuvre</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>le patriotisme économique</t>
+          <t>le protectionnisme intelligent</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>pour donner un</t>
+          <t>la défiscalisation de</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>donner,avantage,entreprises,françaises</t>
+          <t>défiscalisation,heures,supplémentaires,suppression</t>
         </is>
       </c>
     </row>
@@ -464,27 +464,27 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>PME,met,place,patriotisme,économique</t>
+          <t>$,$,$,mettre,œuvre</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>un patriotisme économique</t>
+          <t>en œuvre de</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>un protectionnisme intelligent</t>
+          <t>le protectionnisme intelligent</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>il dit à</t>
+          <t>à mettre en</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>dit,constructeurs,américains,voulez</t>
+          <t>mettre,patriotisme,économique,donner</t>
         </is>
       </c>
     </row>
@@ -494,27 +494,27 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>exclusivement,TPE,PME,met,place</t>
+          <t>mettre,œuvre,protectionnisme,intelligent,mettre</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>met en place</t>
+          <t>en avant de</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>un patriotisme économique</t>
+          <t>le patriotisme économique</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>un protectionnisme intelligent</t>
+          <t>pour donner un</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>protectionnisme,intelligent,dit,constructeurs</t>
+          <t>donner,avantage,entreprises,françaises</t>
         </is>
       </c>
     </row>
@@ -524,27 +524,27 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>$,$,$,mettre,œuvre</t>
+          <t>exclusivement,TPE,PME,met,place</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>en œuvre de</t>
+          <t>met en place</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>le protectionnisme intelligent</t>
+          <t>un patriotisme économique</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>à mettre en</t>
+          <t>un protectionnisme intelligent</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>mettre,patriotisme,économique,donner</t>
+          <t>protectionnisme,intelligent,dit,constructeurs</t>
         </is>
       </c>
     </row>
@@ -600,27 +600,27 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>supplémentaires,suppression,travail,détaché,baisse</t>
+          <t>patriotisme,économique,protectionnisme,intelligent,dit</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>la baisse de</t>
+          <t>il dit à</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>les charges</t>
+          <t>les constructeurs américains</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>mais exclusivement pour</t>
+          <t>si vous voulez</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>exclusivement,TPE,PME,met</t>
+          <t>voulez,aller,faire,voitures</t>
         </is>
       </c>
     </row>
@@ -660,27 +660,27 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>travail,détaché,baisse,charges,exclusivement</t>
+          <t>construire,voiture,étranger,paierez,taxe</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>mais exclusivement pour</t>
+          <t>une taxe en</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>les TPE PME .</t>
+          <t>les réimportant</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Il met en</t>
+          <t>à les Etats-Unis</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>met,place,patriotisme,économique</t>
+          <t>Etats-Unis,autant,évidemment,Trump</t>
         </is>
       </c>
     </row>
@@ -690,27 +690,27 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>patriotisme,économique,protectionnisme,intelligent,dit</t>
+          <t>supplémentaires,suppression,travail,détaché,baisse</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>il dit à</t>
+          <t>la baisse de</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>les constructeurs américains</t>
+          <t>les charges</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>si vous voulez</t>
+          <t>mais exclusivement pour</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>voulez,aller,faire,voitures</t>
+          <t>exclusivement,TPE,PME,met</t>
         </is>
       </c>
     </row>
@@ -750,27 +750,27 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>construire,voiture,étranger,paierez,taxe</t>
+          <t>travail,détaché,baisse,charges,exclusivement</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>une taxe en</t>
+          <t>mais exclusivement pour</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>les réimportant</t>
+          <t>les TPE PME .</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>à les Etats-Unis</t>
+          <t>Il met en</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Etats-Unis,autant,évidemment,Trump</t>
+          <t>met,place,patriotisme,économique</t>
         </is>
       </c>
     </row>
@@ -1024,12 +1024,12 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>intéresse,cause,puisqu,met,place</t>
+          <t>place,politique,appelle,vœux,notamment</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>met en place</t>
+          <t>longtemps et notamment</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
@@ -1039,12 +1039,12 @@
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>que j’ appelle</t>
+          <t>de patriotisme économique</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>appelle,vœux,notamment,politique</t>
+          <t>patriotisme,économique,protectionnisme,intelligent</t>
         </is>
       </c>
     </row>
@@ -1054,12 +1054,12 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>place,politique,appelle,vœux,notamment</t>
+          <t>intéresse,cause,puisqu,met,place</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>longtemps et notamment</t>
+          <t>met en place</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
@@ -1069,12 +1069,12 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>de patriotisme économique</t>
+          <t>que j’ appelle</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>patriotisme,économique,protectionnisme,intelligent</t>
+          <t>appelle,vœux,notamment,politique</t>
         </is>
       </c>
     </row>

</xml_diff>